<commit_message>
Update CR_Review_1&3 to closed
</commit_message>
<xml_diff>
--- a/Input Documents/CR/Review/PO_SAG_CR_WEB_Review.xlsx
+++ b/Input Documents/CR/Review/PO_SAG_CR_WEB_Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Repos\sag\WEB_SWProcess_Documents\Input Documents\CR\Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F04AB0-210D-4BD0-918B-D537C61D1D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795BB8A4-74F5-415D-98FB-F8029802E525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1872" yWindow="1872" windowWidth="12300" windowHeight="6180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Entry Date</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t xml:space="preserve">points 3 &amp; 4 shall be removed </t>
+  </si>
+  <si>
+    <t>Closed</t>
   </si>
 </sst>
 </file>
@@ -502,8 +505,8 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -567,7 +570,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="67.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -619,7 +622,7 @@
         <v>22</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Closing Review points 2 , 8
</commit_message>
<xml_diff>
--- a/Input Documents/CR/Review/PO_SAG_CR_WEB_Review.xlsx
+++ b/Input Documents/CR/Review/PO_SAG_CR_WEB_Review.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Repos\sag\WEB_SWProcess_Documents\Input Documents\CR\Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Repos\SAG\WEB_SWProcess_Documents\Input Documents\CR\Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23ADC7D-88F0-4528-A535-46D2C97DCDBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA2B401-D617-43CF-A3B0-700D898CF897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -520,8 +520,8 @@
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -611,7 +611,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -767,7 +767,7 @@
         <v>45</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Change CR status to released
</commit_message>
<xml_diff>
--- a/Input Documents/CR/Review/PO_SAG_CR_WEB_Review.xlsx
+++ b/Input Documents/CR/Review/PO_SAG_CR_WEB_Review.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mentorship\SAG\WEB_SWProcess_Documents\Input Documents\CR\Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Repos\SAG\WEB_SWProcess_Documents\Input Documents\CR\Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642A4B67-572F-4906-8589-6F17E17BBDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,7 +177,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
@@ -525,14 +526,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -781,7 +782,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="31.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -804,7 +805,7 @@
         <v>49</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -953,7 +954,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>